<commit_message>
Added key vault code
</commit_message>
<xml_diff>
--- a/EmailConfirmationServerCore/wwwroot/TestSheet.xlsx
+++ b/EmailConfirmationServerCore/wwwroot/TestSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20350"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stmartin.edu\dfs\users\zachary.michaels\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimberly.castro\Source\Repos\emailConfirmationAssistant\EmailConfirmationServer\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F41D798-2114-48FE-B09D-3FE9A76A6A8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE3F1B6-FAAE-42C7-B82D-EAE9CC322842}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11010" xr2:uid="{227B31AE-315F-4CFF-8A71-775C54A0AB13}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>kimberly.castro13@outlook.com</t>
   </si>
@@ -96,12 +96,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF90EE90"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,10 +123,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -455,15 +462,15 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.265625" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -477,7 +484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -491,7 +498,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -501,11 +508,11 @@
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Added AzureKeyVault connected service
</commit_message>
<xml_diff>
--- a/EmailConfirmationServerCore/wwwroot/TestSheet.xlsx
+++ b/EmailConfirmationServerCore/wwwroot/TestSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20350"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimberly.castro\Source\Repos\emailConfirmationAssistant\EmailConfirmationServer\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stmartin.edu\dfs\users\zachary.michaels\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE3F1B6-FAAE-42C7-B82D-EAE9CC322842}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F41D798-2114-48FE-B09D-3FE9A76A6A8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11010" xr2:uid="{227B31AE-315F-4CFF-8A71-775C54A0AB13}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
   <si>
     <t>kimberly.castro13@outlook.com</t>
   </si>
@@ -96,18 +96,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF90EE90"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -123,11 +117,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -462,15 +455,15 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="28.265625" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -484,7 +477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -498,7 +491,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -508,11 +501,11 @@
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
added confirm prompt for deleting spreadsheet
</commit_message>
<xml_diff>
--- a/EmailConfirmationServerCore/wwwroot/TestSheet.xlsx
+++ b/EmailConfirmationServerCore/wwwroot/TestSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\Desktop\MSSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74DDDBDD-08D4-4531-A245-607511E34023}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB897DCD-DAF7-464C-86DE-5585A67785A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="2940" windowWidth="23256" windowHeight="12576" xr2:uid="{B8594FB2-BCB3-44B7-BF4E-B5EFBE5AF520}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8594FB2-BCB3-44B7-BF4E-B5EFBE5AF520}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -441,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B09C596-6A11-41E5-A424-5EEE47D7C462}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,14 +510,62 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{485AD91A-6561-4BC6-A7F1-F3B315112724}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{C7845A9D-8189-4EA5-B0EE-49C146D84F56}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{DA1E5233-862D-4FF1-B4BE-95F73F202DAA}"/>
-    <hyperlink ref="D3" r:id="rId4" xr:uid="{E2326F59-D91C-4058-A96D-3743FAE95AAE}"/>
-    <hyperlink ref="C4" r:id="rId5" xr:uid="{19BA37E3-88A3-4C2B-A513-56FB0DE985A6}"/>
-    <hyperlink ref="D4" r:id="rId6" xr:uid="{459B7D74-B08D-4FE8-AE0C-8DEF0458EA16}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{459B7D74-B08D-4FE8-AE0C-8DEF0458EA16}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{19BA37E3-88A3-4C2B-A513-56FB0DE985A6}"/>
+    <hyperlink ref="D3" r:id="rId5" xr:uid="{E2326F59-D91C-4058-A96D-3743FAE95AAE}"/>
+    <hyperlink ref="C3" r:id="rId6" xr:uid="{DA1E5233-862D-4FF1-B4BE-95F73F202DAA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>